<commit_message>
Fixing bug in firmware with TX and RX Amp enable
</commit_message>
<xml_diff>
--- a/Hardware/S-Band Transceiver/BOM_S-Band_Transceiver_v1.0.xlsx
+++ b/Hardware/S-Band Transceiver/BOM_S-Band_Transceiver_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkell\Repositories\openEPR\Hardware\S-Band Transceiver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tkeller\Repositories\openEPR\Hardware\S-Band Transceiver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5A7126BF-3419-4BAF-A077-F9A10E040BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F830A628-424F-4ADB-B829-4AFC8814D732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_S-Band_Transceiver_v1.0" sheetId="1" r:id="rId1"/>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1025,7 +1025,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1039,9 +1039,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1101,18 +1098,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FFC00000"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1450,41 +1440,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1500,11 +1493,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
@@ -1514,11 +1507,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -1528,11 +1521,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
@@ -1542,11 +1535,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C9" t="s">
@@ -1556,11 +1549,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
@@ -1570,11 +1563,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
@@ -1584,11 +1577,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="s">
@@ -1598,11 +1591,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C13" t="s">
@@ -1612,11 +1605,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C14" t="s">
@@ -1626,11 +1619,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C15" t="s">
@@ -1640,11 +1633,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C16" t="s">
@@ -1654,11 +1647,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C17" t="s">
@@ -1668,11 +1661,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C18" t="s">
@@ -1685,11 +1678,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C19" t="s">
@@ -1702,11 +1695,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C20" t="s">
@@ -1716,11 +1709,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C21" t="s">
@@ -1730,11 +1723,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C22" t="s">
@@ -1747,11 +1740,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C23" t="s">
@@ -1761,11 +1754,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <v>14702</v>
       </c>
       <c r="C24" t="s">
@@ -1775,11 +1768,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C25" t="s">
@@ -1792,11 +1785,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C26" t="s">
@@ -1806,11 +1799,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C27" t="s">
@@ -1823,11 +1816,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C28" t="s">
@@ -1837,11 +1830,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C29" t="s">
@@ -1851,11 +1844,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C30" t="s">
@@ -1865,11 +1858,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C31" t="s">
@@ -1879,11 +1872,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="7">
         <v>0</v>
       </c>
       <c r="C32" t="s">
@@ -1893,11 +1886,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C33" t="s">
@@ -1907,11 +1900,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C34" t="s">
@@ -1921,11 +1914,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="7">
         <v>0</v>
       </c>
       <c r="C35" t="s">
@@ -1938,11 +1931,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="7">
         <v>360</v>
       </c>
       <c r="C36" t="s">
@@ -1952,11 +1945,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>82</v>
       </c>
       <c r="C37" t="s">
@@ -1966,11 +1959,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="7">
         <v>27</v>
       </c>
       <c r="C38" t="s">
@@ -1980,11 +1973,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C39" t="s">
@@ -1994,11 +1987,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>87</v>
       </c>
       <c r="C40" t="s">
@@ -2008,11 +2001,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="7">
         <v>60.4</v>
       </c>
       <c r="C41" t="s">
@@ -2022,11 +2015,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7">
         <v>50</v>
       </c>
       <c r="C42" t="s">
@@ -2036,11 +2029,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C43" t="s">
@@ -2050,11 +2043,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
         <v>93</v>
       </c>
       <c r="C44" t="s">
@@ -2064,11 +2057,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <v>270</v>
       </c>
       <c r="C45" t="s">
@@ -2078,11 +2071,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C46" t="s">
@@ -2092,11 +2085,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>200</v>
       </c>
       <c r="C47" t="s">
@@ -2106,11 +2099,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="7">
         <v>430</v>
       </c>
       <c r="C48" t="s">
@@ -2120,11 +2113,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>100</v>
       </c>
       <c r="C49" t="s">
@@ -2134,11 +2127,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C50" t="s">
@@ -2151,11 +2144,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C51" t="s">
@@ -2168,11 +2161,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C52" t="s">
@@ -2185,11 +2178,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="7" t="s">
         <v>115</v>
       </c>
       <c r="C53" t="s">
@@ -2202,11 +2195,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="7" t="s">
         <v>119</v>
       </c>
       <c r="C54" t="s">
@@ -2219,11 +2212,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="7" t="s">
         <v>123</v>
       </c>
       <c r="C55" t="s">
@@ -2236,11 +2229,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="7" t="s">
         <v>127</v>
       </c>
       <c r="C56" t="s">
@@ -2253,11 +2246,11 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="7" t="s">
         <v>131</v>
       </c>
       <c r="C57" t="s">
@@ -2270,11 +2263,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="7" t="s">
         <v>134</v>
       </c>
       <c r="C58" t="s">
@@ -2287,11 +2280,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="7" t="s">
         <v>138</v>
       </c>
       <c r="C59" t="s">
@@ -2304,11 +2297,11 @@
         <v>140</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="7" t="s">
         <v>142</v>
       </c>
       <c r="C60" t="s">
@@ -2321,11 +2314,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="7" t="s">
         <v>146</v>
       </c>
       <c r="C61" t="s">
@@ -2338,11 +2331,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C62" t="s">
@@ -2355,11 +2348,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="7" t="s">
         <v>154</v>
       </c>
       <c r="C63" t="s">
@@ -2372,11 +2365,11 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C64" t="s">
@@ -2389,11 +2382,11 @@
         <v>160</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="7" t="s">
         <v>162</v>
       </c>
       <c r="C65" t="s">
@@ -2406,11 +2399,11 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="B66" s="10" t="s">
         <v>166</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -2422,7 +2415,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:XFD66">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2432,6 +2425,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="47" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>